<commit_message>
doc: Estimativa tamanho e esforco
</commit_message>
<xml_diff>
--- a/PFC_Doc_2022/ApêndiceH-EstimativasdeTamanhoeEsforço/FAI_SI_PFC_Fase2_EstimativaPorCasosdeUso.xlsx
+++ b/PFC_Doc_2022/ApêndiceH-EstimativasdeTamanhoeEsforço/FAI_SI_PFC_Fase2_EstimativaPorCasosdeUso.xlsx
@@ -1,24 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vinicius\Desktop\Deu Pet\Deu-Pet_documments\PFC_Doc_2022\ApêndiceH-EstimativasdeTamanhoeEsforço\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8A2EA72-111C-4155-BE76-CE9906F761F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="516" windowWidth="12120" windowHeight="8448"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PCU-Fase 2" sheetId="16" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'PCU-Fase 2'!$I$31:$I$33</definedName>
-    <definedName name="_xlnm.Extract" localSheetId="0">'PCU-Fase 2'!$I$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'PCU-Fase 2'!$I$32:$I$34</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="0">'PCU-Fase 2'!$I$40</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="128">
   <si>
     <t>Descrição</t>
   </si>
@@ -92,9 +110,6 @@
     <t>Se X + Y &lt;= 2, usar 20 como unidade de homens/hora</t>
   </si>
   <si>
-    <t>Nome do ator</t>
-  </si>
-  <si>
     <t>Nome do caso de uso</t>
   </si>
   <si>
@@ -387,18 +402,36 @@
   </si>
   <si>
     <t>Y = Total de Itens de FA7 a FA8 com valor maior que 3. A contagem deve ser feita na coluna "Valor" da tabela de FA</t>
+  </si>
+  <si>
+    <t>Deu Pet</t>
+  </si>
+  <si>
+    <t>Adotante</t>
+  </si>
+  <si>
+    <t>Interessado campanha</t>
+  </si>
+  <si>
+    <t>Administrador</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Responsavel Instituição </t>
+  </si>
+  <si>
+    <t>Servidor de E-mail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="&quot;R$ &quot;#,##0.00"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1074,121 +1107,31 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1206,6 +1149,9 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1236,9 +1182,96 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1257,7 +1290,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1295,9 +1328,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1329,9 +1362,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1363,9 +1414,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1538,42 +1607,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U124"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:U125"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:D3"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.88671875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.88671875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.88671875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="22.44140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.109375" style="3" hidden="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="26.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="3" hidden="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="32.25" customHeight="1">
-      <c r="A1" s="104" t="s">
-        <v>64</v>
-      </c>
-      <c r="B1" s="104"/>
-      <c r="C1" s="104"/>
-      <c r="D1" s="104"/>
-      <c r="E1" s="104"/>
-      <c r="F1" s="104"/>
-      <c r="G1" s="104"/>
-      <c r="H1" s="104"/>
-      <c r="I1" s="105"/>
-    </row>
-    <row r="2" spans="1:9" ht="23.25" customHeight="1">
+    <row r="1" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="109" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="109"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
+      <c r="G1" s="109"/>
+      <c r="H1" s="109"/>
+      <c r="I1" s="110"/>
+    </row>
+    <row r="2" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="63"/>
       <c r="B2" s="63"/>
       <c r="C2" s="63"/>
@@ -1584,20 +1653,22 @@
       <c r="H2" s="63"/>
       <c r="I2" s="64"/>
     </row>
-    <row r="3" spans="1:9" ht="28.2">
+    <row r="3" spans="1:9" ht="27.75" x14ac:dyDescent="0.4">
       <c r="A3" s="60" t="s">
-        <v>61</v>
-      </c>
-      <c r="B3" s="92"/>
-      <c r="C3" s="93"/>
-      <c r="D3" s="94"/>
+        <v>60</v>
+      </c>
+      <c r="B3" s="116" t="s">
+        <v>122</v>
+      </c>
+      <c r="C3" s="117"/>
+      <c r="D3" s="118"/>
       <c r="E3" s="55"/>
       <c r="F3" s="55"/>
       <c r="G3" s="55"/>
       <c r="H3" s="55"/>
       <c r="I3" s="58"/>
     </row>
-    <row r="4" spans="1:9" ht="28.2">
+    <row r="4" spans="1:9" ht="27.75" x14ac:dyDescent="0.4">
       <c r="A4" s="61"/>
       <c r="B4" s="28"/>
       <c r="C4" s="28"/>
@@ -1608,24 +1679,28 @@
       <c r="H4" s="55"/>
       <c r="I4" s="58"/>
     </row>
-    <row r="5" spans="1:9" ht="17.25" customHeight="1" thickBot="1">
+    <row r="5" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="62" t="s">
-        <v>62</v>
-      </c>
-      <c r="B5" s="56"/>
+        <v>61</v>
+      </c>
+      <c r="B5" s="56">
+        <v>44699</v>
+      </c>
       <c r="C5" s="28"/>
       <c r="D5" s="28"/>
       <c r="E5" s="28"/>
       <c r="F5" s="28"/>
       <c r="G5" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="H5" s="57"/>
+        <v>62</v>
+      </c>
+      <c r="H5" s="57">
+        <v>2</v>
+      </c>
       <c r="I5" s="59"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B6" s="28"/>
       <c r="C6" s="30"/>
@@ -1636,10 +1711,10 @@
       <c r="H6" s="28"/>
       <c r="I6" s="31"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="32"/>
       <c r="B7" s="33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C7" s="28"/>
       <c r="D7" s="28"/>
@@ -1649,10 +1724,10 @@
       <c r="H7" s="28"/>
       <c r="I7" s="34"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="32"/>
       <c r="B8" s="33" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C8" s="28"/>
       <c r="D8" s="28"/>
@@ -1662,10 +1737,10 @@
       <c r="H8" s="28"/>
       <c r="I8" s="34"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="32"/>
       <c r="B9" s="33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C9" s="28"/>
       <c r="D9" s="28"/>
@@ -1675,7 +1750,7 @@
       <c r="H9" s="28"/>
       <c r="I9" s="34"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="32"/>
       <c r="B10" s="33"/>
       <c r="C10" s="28"/>
@@ -1686,10 +1761,10 @@
       <c r="H10" s="28"/>
       <c r="I10" s="34"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="32"/>
       <c r="B11" s="33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C11" s="28"/>
       <c r="D11" s="28"/>
@@ -1699,10 +1774,10 @@
       <c r="H11" s="28"/>
       <c r="I11" s="34"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="32"/>
       <c r="B12" s="33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C12" s="28"/>
       <c r="D12" s="28"/>
@@ -1712,10 +1787,10 @@
       <c r="H12" s="28"/>
       <c r="I12" s="34"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="32"/>
       <c r="B13" s="33" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C13" s="28"/>
       <c r="D13" s="28"/>
@@ -1725,7 +1800,7 @@
       <c r="H13" s="28"/>
       <c r="I13" s="34"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="32"/>
       <c r="B14" s="33"/>
       <c r="C14" s="28"/>
@@ -1736,83 +1811,83 @@
       <c r="H14" s="28"/>
       <c r="I14" s="34"/>
     </row>
-    <row r="15" spans="1:9" ht="13.8" thickBot="1">
+    <row r="15" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="35"/>
       <c r="B15" s="36" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C15" s="69"/>
       <c r="D15" s="56" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E15" s="67" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F15" s="36"/>
       <c r="G15" s="36"/>
       <c r="H15" s="36"/>
       <c r="I15" s="37"/>
     </row>
-    <row r="16" spans="1:9" ht="14.4">
-      <c r="A16" s="106" t="s">
+    <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="111" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="106"/>
-      <c r="C16" s="106"/>
-      <c r="D16" s="106"/>
-      <c r="E16" s="106"/>
-      <c r="F16" s="106"/>
-      <c r="G16" s="106"/>
-      <c r="H16" s="106"/>
-      <c r="I16" s="106"/>
-    </row>
-    <row r="17" spans="1:12" ht="14.4">
+      <c r="B16" s="111"/>
+      <c r="C16" s="111"/>
+      <c r="D16" s="111"/>
+      <c r="E16" s="111"/>
+      <c r="F16" s="111"/>
+      <c r="G16" s="111"/>
+      <c r="H16" s="111"/>
+      <c r="I16" s="111"/>
+    </row>
+    <row r="17" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="70" t="s">
-        <v>101</v>
-      </c>
-      <c r="B17" s="81" t="s">
-        <v>0</v>
-      </c>
-      <c r="C17" s="107"/>
-      <c r="D17" s="107"/>
-      <c r="E17" s="107"/>
-      <c r="F17" s="107"/>
-      <c r="G17" s="107"/>
-      <c r="H17" s="107"/>
+        <v>100</v>
+      </c>
+      <c r="B17" s="112" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="113"/>
+      <c r="D17" s="113"/>
+      <c r="E17" s="113"/>
+      <c r="F17" s="113"/>
+      <c r="G17" s="113"/>
+      <c r="H17" s="113"/>
       <c r="I17" s="38" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="84" t="s">
-        <v>105</v>
-      </c>
-      <c r="C18" s="85"/>
-      <c r="D18" s="85"/>
-      <c r="E18" s="85"/>
-      <c r="F18" s="85"/>
-      <c r="G18" s="85"/>
-      <c r="H18" s="85"/>
+      <c r="B18" s="102" t="s">
+        <v>104</v>
+      </c>
+      <c r="C18" s="82"/>
+      <c r="D18" s="82"/>
+      <c r="E18" s="82"/>
+      <c r="F18" s="82"/>
+      <c r="G18" s="82"/>
+      <c r="H18" s="82"/>
       <c r="I18" s="40">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="84" t="s">
-        <v>107</v>
-      </c>
-      <c r="C19" s="85"/>
-      <c r="D19" s="85"/>
-      <c r="E19" s="85"/>
-      <c r="F19" s="85"/>
-      <c r="G19" s="85"/>
-      <c r="H19" s="85"/>
+      <c r="B19" s="102" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" s="82"/>
+      <c r="D19" s="82"/>
+      <c r="E19" s="82"/>
+      <c r="F19" s="82"/>
+      <c r="G19" s="82"/>
+      <c r="H19" s="82"/>
       <c r="I19" s="40">
         <v>2</v>
       </c>
@@ -1820,19 +1895,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="84" t="s">
-        <v>106</v>
-      </c>
-      <c r="C20" s="85"/>
-      <c r="D20" s="85"/>
-      <c r="E20" s="85"/>
-      <c r="F20" s="85"/>
-      <c r="G20" s="85"/>
-      <c r="H20" s="85"/>
+      <c r="B20" s="102" t="s">
+        <v>105</v>
+      </c>
+      <c r="C20" s="82"/>
+      <c r="D20" s="82"/>
+      <c r="E20" s="82"/>
+      <c r="F20" s="82"/>
+      <c r="G20" s="82"/>
+      <c r="H20" s="82"/>
       <c r="I20" s="40">
         <v>3</v>
       </c>
@@ -1840,7 +1915,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="14.4">
+    <row r="21" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -1856,381 +1931,374 @@
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
     </row>
-    <row r="22" spans="1:12" ht="14.4">
+    <row r="22" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="76" t="s">
+      <c r="B22" s="107" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" s="108"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23" s="52" t="s">
+        <v>123</v>
+      </c>
+      <c r="B23" s="76">
+        <v>3</v>
+      </c>
+      <c r="C23" s="77"/>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24" s="52" t="s">
+        <v>124</v>
+      </c>
+      <c r="B24" s="76">
+        <v>3</v>
+      </c>
+      <c r="C24" s="77"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A25" s="71" t="s">
+        <v>125</v>
+      </c>
+      <c r="B25" s="76">
+        <v>3</v>
+      </c>
+      <c r="C25" s="77"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26" s="52" t="s">
+        <v>126</v>
+      </c>
+      <c r="B26" s="76">
+        <v>3</v>
+      </c>
+      <c r="C26" s="77"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A27" s="75" t="s">
+        <v>127</v>
+      </c>
+      <c r="B27" s="76">
+        <v>1</v>
+      </c>
+      <c r="C27" s="77"/>
+    </row>
+    <row r="28" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="B28" s="122">
+        <f>SUM(B23:C26)</f>
+        <v>12</v>
+      </c>
+      <c r="C28" s="123"/>
+    </row>
+    <row r="29" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="B29" s="8"/>
+      <c r="C29" s="7"/>
+    </row>
+    <row r="30" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30" s="112" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="112"/>
+      <c r="C30" s="112"/>
+      <c r="D30" s="112"/>
+      <c r="E30" s="112"/>
+      <c r="F30" s="112"/>
+      <c r="G30" s="112"/>
+      <c r="H30" s="112"/>
+      <c r="I30" s="112"/>
+    </row>
+    <row r="31" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="70" t="s">
+        <v>101</v>
+      </c>
+      <c r="B31" s="112" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="121"/>
+      <c r="D31" s="121"/>
+      <c r="E31" s="121"/>
+      <c r="F31" s="121"/>
+      <c r="G31" s="121"/>
+      <c r="H31" s="121"/>
+      <c r="I31" s="38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A32" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" s="102" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" s="82"/>
+      <c r="D32" s="82"/>
+      <c r="E32" s="82"/>
+      <c r="F32" s="82"/>
+      <c r="G32" s="82"/>
+      <c r="H32" s="82"/>
+      <c r="I32" s="40">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="102" t="s">
+        <v>76</v>
+      </c>
+      <c r="C33" s="82"/>
+      <c r="D33" s="82"/>
+      <c r="E33" s="82"/>
+      <c r="F33" s="82"/>
+      <c r="G33" s="82"/>
+      <c r="H33" s="82"/>
+      <c r="I33" s="40">
+        <v>10</v>
+      </c>
+      <c r="J33" s="3">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="102" t="s">
+        <v>75</v>
+      </c>
+      <c r="C34" s="82"/>
+      <c r="D34" s="82"/>
+      <c r="E34" s="82"/>
+      <c r="F34" s="82"/>
+      <c r="G34" s="82"/>
+      <c r="H34" s="82"/>
+      <c r="I34" s="40">
+        <v>15</v>
+      </c>
+      <c r="J34" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J35" s="3">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" s="107" t="s">
         <v>73</v>
       </c>
-      <c r="C22" s="77"/>
-    </row>
-    <row r="23" spans="1:12">
-      <c r="A23" s="52" t="s">
+      <c r="C36" s="108"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="97"/>
-      <c r="C23" s="98"/>
-      <c r="D23" s="3"/>
-    </row>
-    <row r="24" spans="1:12">
-      <c r="A24" s="52" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="97"/>
-      <c r="C24" s="98"/>
-    </row>
-    <row r="25" spans="1:12">
-      <c r="A25" s="71" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" s="71"/>
-      <c r="C25" s="72"/>
-    </row>
-    <row r="26" spans="1:12">
-      <c r="A26" s="52" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" s="97"/>
-      <c r="C26" s="98"/>
-    </row>
-    <row r="27" spans="1:12" ht="14.4">
-      <c r="A27" s="41" t="s">
-        <v>99</v>
-      </c>
-      <c r="B27" s="90">
-        <f>SUM(B23:C26)</f>
-        <v>0</v>
-      </c>
-      <c r="C27" s="91"/>
-    </row>
-    <row r="28" spans="1:12" ht="14.4">
-      <c r="B28" s="8"/>
-      <c r="C28" s="7"/>
-    </row>
-    <row r="29" spans="1:12" ht="14.4">
-      <c r="A29" s="81" t="s">
-        <v>7</v>
-      </c>
-      <c r="B29" s="81"/>
-      <c r="C29" s="81"/>
-      <c r="D29" s="81"/>
-      <c r="E29" s="81"/>
-      <c r="F29" s="81"/>
-      <c r="G29" s="81"/>
-      <c r="H29" s="81"/>
-      <c r="I29" s="81"/>
-    </row>
-    <row r="30" spans="1:12" ht="14.4">
-      <c r="A30" s="70" t="s">
-        <v>102</v>
-      </c>
-      <c r="B30" s="81" t="s">
-        <v>0</v>
-      </c>
-      <c r="C30" s="99"/>
-      <c r="D30" s="99"/>
-      <c r="E30" s="99"/>
-      <c r="F30" s="99"/>
-      <c r="G30" s="99"/>
-      <c r="H30" s="99"/>
-      <c r="I30" s="38" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12">
-      <c r="A31" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="B31" s="84" t="s">
-        <v>80</v>
-      </c>
-      <c r="C31" s="85"/>
-      <c r="D31" s="85"/>
-      <c r="E31" s="85"/>
-      <c r="F31" s="85"/>
-      <c r="G31" s="85"/>
-      <c r="H31" s="85"/>
-      <c r="I31" s="40">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12">
-      <c r="A32" s="39" t="s">
-        <v>4</v>
-      </c>
-      <c r="B32" s="84" t="s">
-        <v>77</v>
-      </c>
-      <c r="C32" s="85"/>
-      <c r="D32" s="85"/>
-      <c r="E32" s="85"/>
-      <c r="F32" s="85"/>
-      <c r="G32" s="85"/>
-      <c r="H32" s="85"/>
-      <c r="I32" s="40">
-        <v>10</v>
-      </c>
-      <c r="J32" s="3">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10">
-      <c r="A33" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="B33" s="84" t="s">
-        <v>76</v>
-      </c>
-      <c r="C33" s="85"/>
-      <c r="D33" s="85"/>
-      <c r="E33" s="85"/>
-      <c r="F33" s="85"/>
-      <c r="G33" s="85"/>
-      <c r="H33" s="85"/>
-      <c r="I33" s="40">
-        <v>15</v>
-      </c>
-      <c r="J33" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10">
-      <c r="J34" s="3">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="14.4">
-      <c r="A35" s="70" t="s">
-        <v>8</v>
-      </c>
-      <c r="B35" s="76" t="s">
-        <v>74</v>
-      </c>
-      <c r="C35" s="77"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10">
-      <c r="A36" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="B36" s="78"/>
-      <c r="C36" s="79"/>
-      <c r="D36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="J36" s="3">
-        <v>12.5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10">
-      <c r="A37" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="B37" s="78"/>
-      <c r="C37" s="79"/>
+      <c r="B37" s="114"/>
+      <c r="C37" s="115"/>
+      <c r="D37" s="3"/>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
       <c r="J37" s="3">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="B38" s="78"/>
-      <c r="C38" s="79"/>
+        <v>24</v>
+      </c>
+      <c r="B38" s="114"/>
+      <c r="C38" s="115"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
-    </row>
-    <row r="39" spans="1:10">
+      <c r="J38" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="B39" s="78"/>
-      <c r="C39" s="79"/>
+        <v>24</v>
+      </c>
+      <c r="B39" s="114"/>
+      <c r="C39" s="115"/>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
-    </row>
-    <row r="40" spans="1:10">
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="B40" s="78"/>
-      <c r="C40" s="79"/>
+        <v>24</v>
+      </c>
+      <c r="B40" s="114"/>
+      <c r="C40" s="115"/>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
-    </row>
-    <row r="41" spans="1:10">
+      <c r="I40" s="3"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="B41" s="78"/>
-      <c r="C41" s="79"/>
+        <v>24</v>
+      </c>
+      <c r="B41" s="114"/>
+      <c r="C41" s="115"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="B42" s="78"/>
-      <c r="C42" s="79"/>
+        <v>24</v>
+      </c>
+      <c r="B42" s="114"/>
+      <c r="C42" s="115"/>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="B43" s="78"/>
-      <c r="C43" s="79"/>
+        <v>24</v>
+      </c>
+      <c r="B43" s="114"/>
+      <c r="C43" s="115"/>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="B44" s="78"/>
-      <c r="C44" s="79"/>
+        <v>24</v>
+      </c>
+      <c r="B44" s="114"/>
+      <c r="C44" s="115"/>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="B45" s="78"/>
-      <c r="C45" s="79"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
+        <v>24</v>
+      </c>
+      <c r="B45" s="114"/>
+      <c r="C45" s="115"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
       <c r="H45" s="3"/>
-      <c r="I45" s="3"/>
-    </row>
-    <row r="46" spans="1:10">
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="B46" s="78"/>
-      <c r="C46" s="79"/>
+        <v>24</v>
+      </c>
+      <c r="B46" s="114"/>
+      <c r="C46" s="115"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="B47" s="78"/>
-      <c r="C47" s="79"/>
+        <v>24</v>
+      </c>
+      <c r="B47" s="114"/>
+      <c r="C47" s="115"/>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="B48" s="78"/>
-      <c r="C48" s="79"/>
+        <v>24</v>
+      </c>
+      <c r="B48" s="114"/>
+      <c r="C48" s="115"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
     </row>
-    <row r="49" spans="1:21">
-      <c r="A49" s="41" t="s">
-        <v>100</v>
-      </c>
-      <c r="B49" s="109">
-        <f>SUM(B36:B48)</f>
-        <v>0</v>
-      </c>
-      <c r="C49" s="110"/>
-      <c r="D49" s="3" t="s">
-        <v>9</v>
-      </c>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A49" s="53" t="s">
+        <v>24</v>
+      </c>
+      <c r="B49" s="114"/>
+      <c r="C49" s="115"/>
+      <c r="D49" s="3"/>
       <c r="E49" s="3"/>
-      <c r="F49" s="10"/>
-      <c r="G49" s="3"/>
       <c r="H49" s="3"/>
       <c r="I49" s="3"/>
     </row>
-    <row r="50" spans="1:21">
-      <c r="A50" s="9"/>
-      <c r="B50" s="15"/>
-      <c r="C50" s="15"/>
-      <c r="D50" s="3"/>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A50" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="B50" s="104">
+        <f>SUM(B37:B49)</f>
+        <v>0</v>
+      </c>
+      <c r="C50" s="105"/>
+      <c r="D50" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="E50" s="3"/>
       <c r="F50" s="10"/>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
     </row>
-    <row r="51" spans="1:21" ht="14.4">
-      <c r="A51" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="B51" s="90">
-        <f>B27+B49</f>
-        <v>0</v>
-      </c>
-      <c r="C51" s="91"/>
-    </row>
-    <row r="52" spans="1:21">
-      <c r="A52" s="9"/>
-      <c r="B52" s="9"/>
-      <c r="C52" s="9"/>
-      <c r="D52" s="9"/>
-      <c r="E52" s="9"/>
-      <c r="F52" s="9"/>
-      <c r="G52" s="9"/>
-      <c r="H52" s="9"/>
-      <c r="I52" s="9"/>
-      <c r="K52" s="9"/>
-      <c r="L52" s="9"/>
-      <c r="M52" s="9"/>
-      <c r="N52" s="9"/>
-      <c r="O52" s="9"/>
-      <c r="P52" s="9"/>
-      <c r="Q52" s="9"/>
-      <c r="R52" s="9"/>
-      <c r="S52" s="9"/>
-      <c r="T52" s="9"/>
-      <c r="U52" s="9"/>
-    </row>
-    <row r="53" spans="1:21" ht="14.4">
-      <c r="A53" s="81" t="s">
-        <v>59</v>
-      </c>
-      <c r="B53" s="82"/>
-      <c r="C53" s="82"/>
-      <c r="D53" s="82"/>
-      <c r="E53" s="82"/>
-      <c r="F53" s="82"/>
-      <c r="G53" s="83"/>
-      <c r="H53" s="83"/>
-      <c r="I53" s="83"/>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A51" s="9"/>
+      <c r="B51" s="15"/>
+      <c r="C51" s="15"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="10"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="3"/>
+    </row>
+    <row r="52" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A52" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="B52" s="122">
+        <f>B28+B50</f>
+        <v>12</v>
+      </c>
+      <c r="C52" s="123"/>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A53" s="9"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="9"/>
+      <c r="G53" s="9"/>
+      <c r="H53" s="9"/>
+      <c r="I53" s="9"/>
       <c r="K53" s="9"/>
       <c r="L53" s="9"/>
       <c r="M53" s="9"/>
@@ -2243,18 +2311,18 @@
       <c r="T53" s="9"/>
       <c r="U53" s="9"/>
     </row>
-    <row r="54" spans="1:21">
-      <c r="A54" s="84" t="s">
-        <v>88</v>
-      </c>
-      <c r="B54" s="85"/>
-      <c r="C54" s="85"/>
-      <c r="D54" s="85"/>
-      <c r="E54" s="85"/>
-      <c r="F54" s="85"/>
-      <c r="G54" s="85"/>
-      <c r="H54" s="85"/>
-      <c r="I54" s="85"/>
+    <row r="54" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A54" s="112" t="s">
+        <v>58</v>
+      </c>
+      <c r="B54" s="90"/>
+      <c r="C54" s="90"/>
+      <c r="D54" s="90"/>
+      <c r="E54" s="90"/>
+      <c r="F54" s="90"/>
+      <c r="G54" s="79"/>
+      <c r="H54" s="79"/>
+      <c r="I54" s="79"/>
       <c r="K54" s="9"/>
       <c r="L54" s="9"/>
       <c r="M54" s="9"/>
@@ -2267,18 +2335,18 @@
       <c r="T54" s="9"/>
       <c r="U54" s="9"/>
     </row>
-    <row r="55" spans="1:21">
-      <c r="A55" s="84" t="s">
-        <v>89</v>
-      </c>
-      <c r="B55" s="85"/>
-      <c r="C55" s="85"/>
-      <c r="D55" s="85"/>
-      <c r="E55" s="85"/>
-      <c r="F55" s="85"/>
-      <c r="G55" s="85"/>
-      <c r="H55" s="85"/>
-      <c r="I55" s="85"/>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A55" s="102" t="s">
+        <v>87</v>
+      </c>
+      <c r="B55" s="82"/>
+      <c r="C55" s="82"/>
+      <c r="D55" s="82"/>
+      <c r="E55" s="82"/>
+      <c r="F55" s="82"/>
+      <c r="G55" s="82"/>
+      <c r="H55" s="82"/>
+      <c r="I55" s="82"/>
       <c r="K55" s="9"/>
       <c r="L55" s="9"/>
       <c r="M55" s="9"/>
@@ -2291,18 +2359,18 @@
       <c r="T55" s="9"/>
       <c r="U55" s="9"/>
     </row>
-    <row r="56" spans="1:21">
-      <c r="A56" s="85" t="s">
-        <v>83</v>
-      </c>
-      <c r="B56" s="85"/>
-      <c r="C56" s="85"/>
-      <c r="D56" s="85"/>
-      <c r="E56" s="85"/>
-      <c r="F56" s="85"/>
-      <c r="G56" s="85"/>
-      <c r="H56" s="85"/>
-      <c r="I56" s="85"/>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A56" s="102" t="s">
+        <v>88</v>
+      </c>
+      <c r="B56" s="82"/>
+      <c r="C56" s="82"/>
+      <c r="D56" s="82"/>
+      <c r="E56" s="82"/>
+      <c r="F56" s="82"/>
+      <c r="G56" s="82"/>
+      <c r="H56" s="82"/>
+      <c r="I56" s="82"/>
       <c r="K56" s="9"/>
       <c r="L56" s="9"/>
       <c r="M56" s="9"/>
@@ -2315,18 +2383,18 @@
       <c r="T56" s="9"/>
       <c r="U56" s="9"/>
     </row>
-    <row r="57" spans="1:21">
-      <c r="A57" s="85" t="s">
-        <v>84</v>
-      </c>
-      <c r="B57" s="83"/>
-      <c r="C57" s="83"/>
-      <c r="D57" s="83"/>
-      <c r="E57" s="83"/>
-      <c r="F57" s="83"/>
-      <c r="G57" s="83"/>
-      <c r="H57" s="83"/>
-      <c r="I57" s="83"/>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A57" s="82" t="s">
+        <v>82</v>
+      </c>
+      <c r="B57" s="82"/>
+      <c r="C57" s="82"/>
+      <c r="D57" s="82"/>
+      <c r="E57" s="82"/>
+      <c r="F57" s="82"/>
+      <c r="G57" s="82"/>
+      <c r="H57" s="82"/>
+      <c r="I57" s="82"/>
       <c r="K57" s="9"/>
       <c r="L57" s="9"/>
       <c r="M57" s="9"/>
@@ -2339,26 +2407,18 @@
       <c r="T57" s="9"/>
       <c r="U57" s="9"/>
     </row>
-    <row r="58" spans="1:21" ht="14.4">
-      <c r="A58" s="73" t="s">
-        <v>119</v>
-      </c>
-      <c r="B58" s="80" t="s">
-        <v>0</v>
-      </c>
-      <c r="C58" s="80"/>
-      <c r="D58" s="80"/>
-      <c r="E58" s="80"/>
-      <c r="F58" s="42" t="s">
-        <v>2</v>
-      </c>
-      <c r="G58" s="42" t="s">
-        <v>10</v>
-      </c>
-      <c r="H58" s="81" t="s">
-        <v>57</v>
-      </c>
-      <c r="I58" s="81"/>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A58" s="82" t="s">
+        <v>83</v>
+      </c>
+      <c r="B58" s="79"/>
+      <c r="C58" s="79"/>
+      <c r="D58" s="79"/>
+      <c r="E58" s="79"/>
+      <c r="F58" s="79"/>
+      <c r="G58" s="79"/>
+      <c r="H58" s="79"/>
+      <c r="I58" s="79"/>
       <c r="K58" s="9"/>
       <c r="L58" s="9"/>
       <c r="M58" s="9"/>
@@ -2371,27 +2431,26 @@
       <c r="T58" s="9"/>
       <c r="U58" s="9"/>
     </row>
-    <row r="59" spans="1:21">
-      <c r="A59" s="40" t="s">
-        <v>27</v>
-      </c>
-      <c r="B59" s="85" t="s">
-        <v>95</v>
-      </c>
-      <c r="C59" s="85"/>
-      <c r="D59" s="85"/>
-      <c r="E59" s="85"/>
-      <c r="F59" s="40">
+    <row r="59" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A59" s="72" t="s">
+        <v>118</v>
+      </c>
+      <c r="B59" s="128" t="s">
+        <v>0</v>
+      </c>
+      <c r="C59" s="128"/>
+      <c r="D59" s="128"/>
+      <c r="E59" s="128"/>
+      <c r="F59" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="G59" s="51">
-        <v>0</v>
-      </c>
-      <c r="H59" s="86">
-        <f>F59*G59</f>
-        <v>0</v>
-      </c>
-      <c r="I59" s="86"/>
+      <c r="G59" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="H59" s="112" t="s">
+        <v>56</v>
+      </c>
+      <c r="I59" s="112"/>
       <c r="K59" s="9"/>
       <c r="L59" s="9"/>
       <c r="M59" s="9"/>
@@ -2404,27 +2463,27 @@
       <c r="T59" s="9"/>
       <c r="U59" s="9"/>
     </row>
-    <row r="60" spans="1:21">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A60" s="40" t="s">
-        <v>28</v>
-      </c>
-      <c r="B60" s="85" t="s">
-        <v>11</v>
-      </c>
-      <c r="C60" s="85"/>
-      <c r="D60" s="85"/>
-      <c r="E60" s="85"/>
+        <v>26</v>
+      </c>
+      <c r="B60" s="82" t="s">
+        <v>94</v>
+      </c>
+      <c r="C60" s="82"/>
+      <c r="D60" s="82"/>
+      <c r="E60" s="82"/>
       <c r="F60" s="40">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G60" s="51">
         <v>0</v>
       </c>
-      <c r="H60" s="86">
-        <f t="shared" ref="H60:H71" si="0">F60*G60</f>
-        <v>0</v>
-      </c>
-      <c r="I60" s="86"/>
+      <c r="H60" s="101">
+        <f>F60*G60</f>
+        <v>0</v>
+      </c>
+      <c r="I60" s="101"/>
       <c r="K60" s="9"/>
       <c r="L60" s="9"/>
       <c r="M60" s="9"/>
@@ -2437,27 +2496,27 @@
       <c r="T60" s="9"/>
       <c r="U60" s="9"/>
     </row>
-    <row r="61" spans="1:21">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A61" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="B61" s="84" t="s">
-        <v>78</v>
-      </c>
-      <c r="C61" s="85"/>
-      <c r="D61" s="85"/>
-      <c r="E61" s="85"/>
+        <v>27</v>
+      </c>
+      <c r="B61" s="82" t="s">
+        <v>11</v>
+      </c>
+      <c r="C61" s="82"/>
+      <c r="D61" s="82"/>
+      <c r="E61" s="82"/>
       <c r="F61" s="40">
         <v>1</v>
       </c>
       <c r="G61" s="51">
         <v>0</v>
       </c>
-      <c r="H61" s="86">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I61" s="86"/>
+      <c r="H61" s="101">
+        <f t="shared" ref="H61:H72" si="0">F61*G61</f>
+        <v>0</v>
+      </c>
+      <c r="I61" s="101"/>
       <c r="K61" s="9"/>
       <c r="L61" s="9"/>
       <c r="M61" s="9"/>
@@ -2470,27 +2529,27 @@
       <c r="T61" s="9"/>
       <c r="U61" s="9"/>
     </row>
-    <row r="62" spans="1:21">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A62" s="40" t="s">
-        <v>30</v>
-      </c>
-      <c r="B62" s="85" t="s">
-        <v>12</v>
-      </c>
-      <c r="C62" s="85"/>
-      <c r="D62" s="85"/>
-      <c r="E62" s="85"/>
+        <v>28</v>
+      </c>
+      <c r="B62" s="102" t="s">
+        <v>77</v>
+      </c>
+      <c r="C62" s="82"/>
+      <c r="D62" s="82"/>
+      <c r="E62" s="82"/>
       <c r="F62" s="40">
         <v>1</v>
       </c>
       <c r="G62" s="51">
         <v>0</v>
       </c>
-      <c r="H62" s="86">
-        <f>F62*G62</f>
-        <v>0</v>
-      </c>
-      <c r="I62" s="86"/>
+      <c r="H62" s="101">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I62" s="101"/>
       <c r="K62" s="9"/>
       <c r="L62" s="9"/>
       <c r="M62" s="9"/>
@@ -2503,30 +2562,30 @@
       <c r="T62" s="9"/>
       <c r="U62" s="9"/>
     </row>
-    <row r="63" spans="1:21">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A63" s="40" t="s">
-        <v>31</v>
-      </c>
-      <c r="B63" s="85" t="s">
-        <v>93</v>
-      </c>
-      <c r="C63" s="85"/>
-      <c r="D63" s="85"/>
-      <c r="E63" s="85"/>
+        <v>29</v>
+      </c>
+      <c r="B63" s="82" t="s">
+        <v>12</v>
+      </c>
+      <c r="C63" s="82"/>
+      <c r="D63" s="82"/>
+      <c r="E63" s="82"/>
       <c r="F63" s="40">
         <v>1</v>
       </c>
       <c r="G63" s="51">
         <v>0</v>
       </c>
-      <c r="H63" s="86">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I63" s="86"/>
+      <c r="H63" s="101">
+        <f>F63*G63</f>
+        <v>0</v>
+      </c>
+      <c r="I63" s="101"/>
       <c r="K63" s="9"/>
       <c r="L63" s="9"/>
-      <c r="M63" s="11"/>
+      <c r="M63" s="9"/>
       <c r="N63" s="9"/>
       <c r="O63" s="9"/>
       <c r="P63" s="9"/>
@@ -2536,30 +2595,30 @@
       <c r="T63" s="9"/>
       <c r="U63" s="9"/>
     </row>
-    <row r="64" spans="1:21">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A64" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="B64" s="85" t="s">
-        <v>13</v>
-      </c>
-      <c r="C64" s="85"/>
-      <c r="D64" s="85"/>
-      <c r="E64" s="85"/>
+        <v>30</v>
+      </c>
+      <c r="B64" s="82" t="s">
+        <v>92</v>
+      </c>
+      <c r="C64" s="82"/>
+      <c r="D64" s="82"/>
+      <c r="E64" s="82"/>
       <c r="F64" s="40">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="G64" s="51">
         <v>0</v>
       </c>
-      <c r="H64" s="86">
+      <c r="H64" s="101">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I64" s="86"/>
+      <c r="I64" s="101"/>
       <c r="K64" s="9"/>
       <c r="L64" s="9"/>
-      <c r="M64" s="9"/>
+      <c r="M64" s="11"/>
       <c r="N64" s="9"/>
       <c r="O64" s="9"/>
       <c r="P64" s="9"/>
@@ -2569,27 +2628,27 @@
       <c r="T64" s="9"/>
       <c r="U64" s="9"/>
     </row>
-    <row r="65" spans="1:21">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A65" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="B65" s="85" t="s">
-        <v>85</v>
-      </c>
-      <c r="C65" s="85"/>
-      <c r="D65" s="85"/>
-      <c r="E65" s="85"/>
+        <v>31</v>
+      </c>
+      <c r="B65" s="82" t="s">
+        <v>13</v>
+      </c>
+      <c r="C65" s="82"/>
+      <c r="D65" s="82"/>
+      <c r="E65" s="82"/>
       <c r="F65" s="40">
         <v>0.5</v>
       </c>
       <c r="G65" s="51">
         <v>0</v>
       </c>
-      <c r="H65" s="86">
+      <c r="H65" s="101">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I65" s="86"/>
+      <c r="I65" s="101"/>
       <c r="K65" s="9"/>
       <c r="L65" s="9"/>
       <c r="M65" s="9"/>
@@ -2602,27 +2661,27 @@
       <c r="T65" s="9"/>
       <c r="U65" s="9"/>
     </row>
-    <row r="66" spans="1:21">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A66" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="B66" s="85" t="s">
-        <v>14</v>
-      </c>
-      <c r="C66" s="85"/>
-      <c r="D66" s="85"/>
-      <c r="E66" s="85"/>
+        <v>32</v>
+      </c>
+      <c r="B66" s="82" t="s">
+        <v>84</v>
+      </c>
+      <c r="C66" s="82"/>
+      <c r="D66" s="82"/>
+      <c r="E66" s="82"/>
       <c r="F66" s="40">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="G66" s="51">
         <v>0</v>
       </c>
-      <c r="H66" s="86">
+      <c r="H66" s="101">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I66" s="86"/>
+      <c r="I66" s="101"/>
       <c r="K66" s="9"/>
       <c r="L66" s="9"/>
       <c r="M66" s="9"/>
@@ -2635,27 +2694,27 @@
       <c r="T66" s="9"/>
       <c r="U66" s="9"/>
     </row>
-    <row r="67" spans="1:21">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A67" s="40" t="s">
-        <v>35</v>
-      </c>
-      <c r="B67" s="85" t="s">
-        <v>94</v>
-      </c>
-      <c r="C67" s="85"/>
-      <c r="D67" s="85"/>
-      <c r="E67" s="85"/>
+        <v>33</v>
+      </c>
+      <c r="B67" s="82" t="s">
+        <v>14</v>
+      </c>
+      <c r="C67" s="82"/>
+      <c r="D67" s="82"/>
+      <c r="E67" s="82"/>
       <c r="F67" s="40">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G67" s="51">
         <v>0</v>
       </c>
-      <c r="H67" s="86">
+      <c r="H67" s="101">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I67" s="86"/>
+      <c r="I67" s="101"/>
       <c r="K67" s="9"/>
       <c r="L67" s="9"/>
       <c r="M67" s="9"/>
@@ -2668,27 +2727,27 @@
       <c r="T67" s="9"/>
       <c r="U67" s="9"/>
     </row>
-    <row r="68" spans="1:21">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A68" s="40" t="s">
-        <v>36</v>
-      </c>
-      <c r="B68" s="85" t="s">
-        <v>15</v>
-      </c>
-      <c r="C68" s="85"/>
-      <c r="D68" s="85"/>
-      <c r="E68" s="85"/>
+        <v>34</v>
+      </c>
+      <c r="B68" s="82" t="s">
+        <v>93</v>
+      </c>
+      <c r="C68" s="82"/>
+      <c r="D68" s="82"/>
+      <c r="E68" s="82"/>
       <c r="F68" s="40">
         <v>1</v>
       </c>
       <c r="G68" s="51">
         <v>0</v>
       </c>
-      <c r="H68" s="86">
+      <c r="H68" s="101">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I68" s="86"/>
+      <c r="I68" s="101"/>
       <c r="K68" s="9"/>
       <c r="L68" s="9"/>
       <c r="M68" s="9"/>
@@ -2701,27 +2760,27 @@
       <c r="T68" s="9"/>
       <c r="U68" s="9"/>
     </row>
-    <row r="69" spans="1:21">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A69" s="40" t="s">
-        <v>37</v>
-      </c>
-      <c r="B69" s="85" t="s">
-        <v>26</v>
-      </c>
-      <c r="C69" s="85"/>
-      <c r="D69" s="85"/>
-      <c r="E69" s="85"/>
+        <v>35</v>
+      </c>
+      <c r="B69" s="82" t="s">
+        <v>15</v>
+      </c>
+      <c r="C69" s="82"/>
+      <c r="D69" s="82"/>
+      <c r="E69" s="82"/>
       <c r="F69" s="40">
         <v>1</v>
       </c>
       <c r="G69" s="51">
         <v>0</v>
       </c>
-      <c r="H69" s="86">
+      <c r="H69" s="101">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I69" s="86"/>
+      <c r="I69" s="101"/>
       <c r="K69" s="9"/>
       <c r="L69" s="9"/>
       <c r="M69" s="9"/>
@@ -2734,27 +2793,27 @@
       <c r="T69" s="9"/>
       <c r="U69" s="9"/>
     </row>
-    <row r="70" spans="1:21">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A70" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="B70" s="85" t="s">
-        <v>86</v>
-      </c>
-      <c r="C70" s="85"/>
-      <c r="D70" s="85"/>
-      <c r="E70" s="85"/>
+        <v>36</v>
+      </c>
+      <c r="B70" s="82" t="s">
+        <v>25</v>
+      </c>
+      <c r="C70" s="82"/>
+      <c r="D70" s="82"/>
+      <c r="E70" s="82"/>
       <c r="F70" s="40">
         <v>1</v>
       </c>
       <c r="G70" s="51">
         <v>0</v>
       </c>
-      <c r="H70" s="86">
+      <c r="H70" s="101">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I70" s="86"/>
+      <c r="I70" s="101"/>
       <c r="K70" s="9"/>
       <c r="L70" s="9"/>
       <c r="M70" s="9"/>
@@ -2767,27 +2826,27 @@
       <c r="T70" s="9"/>
       <c r="U70" s="9"/>
     </row>
-    <row r="71" spans="1:21">
+    <row r="71" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A71" s="40" t="s">
-        <v>39</v>
-      </c>
-      <c r="B71" s="85" t="s">
-        <v>87</v>
-      </c>
-      <c r="C71" s="85"/>
-      <c r="D71" s="85"/>
-      <c r="E71" s="85"/>
+        <v>37</v>
+      </c>
+      <c r="B71" s="82" t="s">
+        <v>85</v>
+      </c>
+      <c r="C71" s="82"/>
+      <c r="D71" s="82"/>
+      <c r="E71" s="82"/>
       <c r="F71" s="40">
         <v>1</v>
       </c>
       <c r="G71" s="51">
         <v>0</v>
       </c>
-      <c r="H71" s="86">
+      <c r="H71" s="101">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I71" s="86"/>
+      <c r="I71" s="101"/>
       <c r="K71" s="9"/>
       <c r="L71" s="9"/>
       <c r="M71" s="9"/>
@@ -2800,21 +2859,27 @@
       <c r="T71" s="9"/>
       <c r="U71" s="9"/>
     </row>
-    <row r="72" spans="1:21" ht="14.4">
-      <c r="A72" s="87" t="s">
-        <v>51</v>
-      </c>
-      <c r="B72" s="88"/>
-      <c r="C72" s="88"/>
-      <c r="D72" s="88"/>
-      <c r="E72" s="88"/>
-      <c r="F72" s="88"/>
-      <c r="G72" s="89"/>
-      <c r="H72" s="90">
-        <f>0.6+(0.01*(SUM(H59:I71)))</f>
-        <v>0.6</v>
-      </c>
-      <c r="I72" s="91"/>
+    <row r="72" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A72" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="B72" s="82" t="s">
+        <v>86</v>
+      </c>
+      <c r="C72" s="82"/>
+      <c r="D72" s="82"/>
+      <c r="E72" s="82"/>
+      <c r="F72" s="40">
+        <v>1</v>
+      </c>
+      <c r="G72" s="51">
+        <v>0</v>
+      </c>
+      <c r="H72" s="101">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I72" s="101"/>
       <c r="K72" s="9"/>
       <c r="L72" s="9"/>
       <c r="M72" s="9"/>
@@ -2827,15 +2892,21 @@
       <c r="T72" s="9"/>
       <c r="U72" s="9"/>
     </row>
-    <row r="73" spans="1:21">
-      <c r="B73" s="9"/>
-      <c r="C73" s="9"/>
-      <c r="D73" s="9"/>
-      <c r="E73" s="9"/>
-      <c r="F73" s="9"/>
-      <c r="G73" s="9"/>
-      <c r="H73" s="9"/>
-      <c r="I73" s="9"/>
+    <row r="73" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A73" s="129" t="s">
+        <v>50</v>
+      </c>
+      <c r="B73" s="130"/>
+      <c r="C73" s="130"/>
+      <c r="D73" s="130"/>
+      <c r="E73" s="130"/>
+      <c r="F73" s="130"/>
+      <c r="G73" s="131"/>
+      <c r="H73" s="122">
+        <f>0.6+(0.01*(SUM(H60:I72)))</f>
+        <v>0.6</v>
+      </c>
+      <c r="I73" s="123"/>
       <c r="K73" s="9"/>
       <c r="L73" s="9"/>
       <c r="M73" s="9"/>
@@ -2848,18 +2919,15 @@
       <c r="T73" s="9"/>
       <c r="U73" s="9"/>
     </row>
-    <row r="74" spans="1:21" ht="14.4">
-      <c r="A74" s="81" t="s">
-        <v>118</v>
-      </c>
-      <c r="B74" s="82"/>
-      <c r="C74" s="82"/>
-      <c r="D74" s="82"/>
-      <c r="E74" s="83"/>
-      <c r="F74" s="83"/>
-      <c r="G74" s="83"/>
-      <c r="H74" s="83"/>
-      <c r="I74" s="83"/>
+    <row r="74" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B74" s="9"/>
+      <c r="C74" s="9"/>
+      <c r="D74" s="9"/>
+      <c r="E74" s="9"/>
+      <c r="F74" s="9"/>
+      <c r="G74" s="9"/>
+      <c r="H74" s="9"/>
+      <c r="I74" s="9"/>
       <c r="K74" s="9"/>
       <c r="L74" s="9"/>
       <c r="M74" s="9"/>
@@ -2872,18 +2940,18 @@
       <c r="T74" s="9"/>
       <c r="U74" s="9"/>
     </row>
-    <row r="75" spans="1:21">
-      <c r="A75" s="84" t="s">
-        <v>88</v>
-      </c>
-      <c r="B75" s="85"/>
-      <c r="C75" s="85"/>
-      <c r="D75" s="85"/>
-      <c r="E75" s="85"/>
-      <c r="F75" s="85"/>
-      <c r="G75" s="85"/>
-      <c r="H75" s="85"/>
-      <c r="I75" s="85"/>
+    <row r="75" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A75" s="112" t="s">
+        <v>117</v>
+      </c>
+      <c r="B75" s="90"/>
+      <c r="C75" s="90"/>
+      <c r="D75" s="90"/>
+      <c r="E75" s="79"/>
+      <c r="F75" s="79"/>
+      <c r="G75" s="79"/>
+      <c r="H75" s="79"/>
+      <c r="I75" s="79"/>
       <c r="K75" s="9"/>
       <c r="L75" s="9"/>
       <c r="M75" s="9"/>
@@ -2896,18 +2964,18 @@
       <c r="T75" s="9"/>
       <c r="U75" s="9"/>
     </row>
-    <row r="76" spans="1:21">
-      <c r="A76" s="85" t="s">
-        <v>113</v>
-      </c>
-      <c r="B76" s="85"/>
-      <c r="C76" s="85"/>
-      <c r="D76" s="85"/>
-      <c r="E76" s="85"/>
-      <c r="F76" s="85"/>
-      <c r="G76" s="85"/>
-      <c r="H76" s="83"/>
-      <c r="I76" s="83"/>
+    <row r="76" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A76" s="102" t="s">
+        <v>87</v>
+      </c>
+      <c r="B76" s="82"/>
+      <c r="C76" s="82"/>
+      <c r="D76" s="82"/>
+      <c r="E76" s="82"/>
+      <c r="F76" s="82"/>
+      <c r="G76" s="82"/>
+      <c r="H76" s="82"/>
+      <c r="I76" s="82"/>
       <c r="K76" s="9"/>
       <c r="L76" s="9"/>
       <c r="M76" s="9"/>
@@ -2920,18 +2988,18 @@
       <c r="T76" s="9"/>
       <c r="U76" s="9"/>
     </row>
-    <row r="77" spans="1:21">
-      <c r="A77" s="85" t="s">
-        <v>114</v>
-      </c>
-      <c r="B77" s="85"/>
-      <c r="C77" s="85"/>
-      <c r="D77" s="85"/>
-      <c r="E77" s="85"/>
-      <c r="F77" s="85"/>
-      <c r="G77" s="85"/>
-      <c r="H77" s="83"/>
-      <c r="I77" s="83"/>
+    <row r="77" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A77" s="82" t="s">
+        <v>112</v>
+      </c>
+      <c r="B77" s="82"/>
+      <c r="C77" s="82"/>
+      <c r="D77" s="82"/>
+      <c r="E77" s="82"/>
+      <c r="F77" s="82"/>
+      <c r="G77" s="82"/>
+      <c r="H77" s="79"/>
+      <c r="I77" s="79"/>
       <c r="K77" s="9"/>
       <c r="L77" s="9"/>
       <c r="M77" s="9"/>
@@ -2944,18 +3012,18 @@
       <c r="T77" s="9"/>
       <c r="U77" s="9"/>
     </row>
-    <row r="78" spans="1:21">
-      <c r="A78" s="85" t="s">
-        <v>115</v>
-      </c>
-      <c r="B78" s="83"/>
-      <c r="C78" s="83"/>
-      <c r="D78" s="83"/>
-      <c r="E78" s="83"/>
-      <c r="F78" s="83"/>
-      <c r="G78" s="83"/>
-      <c r="H78" s="83"/>
-      <c r="I78" s="83"/>
+    <row r="78" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A78" s="82" t="s">
+        <v>113</v>
+      </c>
+      <c r="B78" s="82"/>
+      <c r="C78" s="82"/>
+      <c r="D78" s="82"/>
+      <c r="E78" s="82"/>
+      <c r="F78" s="82"/>
+      <c r="G78" s="82"/>
+      <c r="H78" s="79"/>
+      <c r="I78" s="79"/>
       <c r="K78" s="9"/>
       <c r="L78" s="9"/>
       <c r="M78" s="9"/>
@@ -2968,26 +3036,18 @@
       <c r="T78" s="9"/>
       <c r="U78" s="9"/>
     </row>
-    <row r="79" spans="1:21" ht="14.4">
-      <c r="A79" s="73" t="s">
-        <v>120</v>
-      </c>
-      <c r="B79" s="80" t="s">
-        <v>0</v>
-      </c>
-      <c r="C79" s="85"/>
-      <c r="D79" s="85"/>
-      <c r="E79" s="85"/>
-      <c r="F79" s="85"/>
-      <c r="G79" s="42" t="s">
-        <v>2</v>
-      </c>
-      <c r="H79" s="42" t="s">
-        <v>10</v>
-      </c>
-      <c r="I79" s="38" t="s">
-        <v>57</v>
-      </c>
+    <row r="79" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A79" s="82" t="s">
+        <v>114</v>
+      </c>
+      <c r="B79" s="79"/>
+      <c r="C79" s="79"/>
+      <c r="D79" s="79"/>
+      <c r="E79" s="79"/>
+      <c r="F79" s="79"/>
+      <c r="G79" s="79"/>
+      <c r="H79" s="79"/>
+      <c r="I79" s="79"/>
       <c r="K79" s="9"/>
       <c r="L79" s="9"/>
       <c r="M79" s="9"/>
@@ -3000,30 +3060,25 @@
       <c r="T79" s="9"/>
       <c r="U79" s="9"/>
     </row>
-    <row r="80" spans="1:21">
-      <c r="A80" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="B80" s="85" t="s">
-        <v>16</v>
-      </c>
-      <c r="C80" s="85"/>
-      <c r="D80" s="85"/>
-      <c r="E80" s="85"/>
-      <c r="F80" s="85"/>
-      <c r="G80" s="40">
-        <v>1.5</v>
-      </c>
-      <c r="H80" s="51">
-        <v>0</v>
-      </c>
-      <c r="I80" s="16">
-        <f>G80*H80</f>
-        <v>0</v>
-      </c>
-      <c r="J80" s="3">
-        <f t="shared" ref="J80:J85" si="1">IF(H80&lt;3,1,0)</f>
-        <v>1</v>
+    <row r="80" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A80" s="72" t="s">
+        <v>119</v>
+      </c>
+      <c r="B80" s="128" t="s">
+        <v>0</v>
+      </c>
+      <c r="C80" s="82"/>
+      <c r="D80" s="82"/>
+      <c r="E80" s="82"/>
+      <c r="F80" s="82"/>
+      <c r="G80" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="H80" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="I80" s="38" t="s">
+        <v>56</v>
       </c>
       <c r="K80" s="9"/>
       <c r="L80" s="9"/>
@@ -3037,51 +3092,62 @@
       <c r="T80" s="9"/>
       <c r="U80" s="9"/>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A81" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="B81" s="84" t="s">
-        <v>79</v>
-      </c>
-      <c r="C81" s="85"/>
-      <c r="D81" s="85"/>
-      <c r="E81" s="85"/>
-      <c r="F81" s="85"/>
+        <v>39</v>
+      </c>
+      <c r="B81" s="82" t="s">
+        <v>16</v>
+      </c>
+      <c r="C81" s="82"/>
+      <c r="D81" s="82"/>
+      <c r="E81" s="82"/>
+      <c r="F81" s="82"/>
       <c r="G81" s="40">
+        <v>1.5</v>
+      </c>
+      <c r="H81" s="51">
+        <v>0</v>
+      </c>
+      <c r="I81" s="16">
+        <f>G81*H81</f>
+        <v>0</v>
+      </c>
+      <c r="J81" s="3">
+        <f t="shared" ref="J81:J86" si="1">IF(H81&lt;3,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="K81" s="9"/>
+      <c r="L81" s="9"/>
+      <c r="M81" s="9"/>
+      <c r="N81" s="9"/>
+      <c r="O81" s="9"/>
+      <c r="P81" s="9"/>
+      <c r="Q81" s="9"/>
+      <c r="R81" s="9"/>
+      <c r="S81" s="9"/>
+      <c r="T81" s="9"/>
+      <c r="U81" s="9"/>
+    </row>
+    <row r="82" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A82" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="B82" s="102" t="s">
+        <v>78</v>
+      </c>
+      <c r="C82" s="82"/>
+      <c r="D82" s="82"/>
+      <c r="E82" s="82"/>
+      <c r="F82" s="82"/>
+      <c r="G82" s="40">
         <v>0.5</v>
       </c>
-      <c r="H81" s="51">
-        <v>0</v>
-      </c>
-      <c r="I81" s="16">
-        <f t="shared" ref="I81:I87" si="2">G81*H81</f>
-        <v>0</v>
-      </c>
-      <c r="J81" s="3">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10">
-      <c r="A82" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="B82" s="85" t="s">
-        <v>81</v>
-      </c>
-      <c r="C82" s="85"/>
-      <c r="D82" s="85"/>
-      <c r="E82" s="85"/>
-      <c r="F82" s="85"/>
-      <c r="G82" s="40">
-        <v>1</v>
-      </c>
       <c r="H82" s="51">
         <v>0</v>
       </c>
       <c r="I82" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="I82:I88" si="2">G82*H82</f>
         <v>0</v>
       </c>
       <c r="J82" s="3">
@@ -3089,19 +3155,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A83" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="B83" s="85" t="s">
-        <v>92</v>
-      </c>
-      <c r="C83" s="85"/>
-      <c r="D83" s="85"/>
-      <c r="E83" s="85"/>
-      <c r="F83" s="85"/>
+        <v>41</v>
+      </c>
+      <c r="B83" s="82" t="s">
+        <v>80</v>
+      </c>
+      <c r="C83" s="82"/>
+      <c r="D83" s="82"/>
+      <c r="E83" s="82"/>
+      <c r="F83" s="82"/>
       <c r="G83" s="40">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H83" s="51">
         <v>0</v>
@@ -3115,19 +3181,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A84" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="B84" s="85" t="s">
-        <v>17</v>
-      </c>
-      <c r="C84" s="85"/>
-      <c r="D84" s="85"/>
-      <c r="E84" s="85"/>
-      <c r="F84" s="85"/>
+        <v>42</v>
+      </c>
+      <c r="B84" s="82" t="s">
+        <v>91</v>
+      </c>
+      <c r="C84" s="82"/>
+      <c r="D84" s="82"/>
+      <c r="E84" s="82"/>
+      <c r="F84" s="82"/>
       <c r="G84" s="40">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H84" s="51">
         <v>0</v>
@@ -3141,19 +3207,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A85" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="B85" s="100" t="s">
-        <v>56</v>
-      </c>
-      <c r="C85" s="85"/>
-      <c r="D85" s="85"/>
-      <c r="E85" s="85"/>
-      <c r="F85" s="85"/>
+        <v>43</v>
+      </c>
+      <c r="B85" s="82" t="s">
+        <v>17</v>
+      </c>
+      <c r="C85" s="82"/>
+      <c r="D85" s="82"/>
+      <c r="E85" s="82"/>
+      <c r="F85" s="82"/>
       <c r="G85" s="40">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H85" s="51">
         <v>0</v>
@@ -3167,19 +3233,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A86" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="B86" s="85" t="s">
-        <v>18</v>
-      </c>
-      <c r="C86" s="85"/>
-      <c r="D86" s="85"/>
-      <c r="E86" s="85"/>
-      <c r="F86" s="85"/>
+        <v>44</v>
+      </c>
+      <c r="B86" s="124" t="s">
+        <v>55</v>
+      </c>
+      <c r="C86" s="82"/>
+      <c r="D86" s="82"/>
+      <c r="E86" s="82"/>
+      <c r="F86" s="82"/>
       <c r="G86" s="40">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="H86" s="51">
         <v>0</v>
@@ -3189,21 +3255,21 @@
         <v>0</v>
       </c>
       <c r="J86" s="3">
-        <f>IF(H86&gt;3,1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A87" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="B87" s="85" t="s">
-        <v>82</v>
-      </c>
-      <c r="C87" s="85"/>
-      <c r="D87" s="85"/>
-      <c r="E87" s="85"/>
-      <c r="F87" s="85"/>
+        <v>45</v>
+      </c>
+      <c r="B87" s="82" t="s">
+        <v>18</v>
+      </c>
+      <c r="C87" s="82"/>
+      <c r="D87" s="82"/>
+      <c r="E87" s="82"/>
+      <c r="F87" s="82"/>
       <c r="G87" s="40">
         <v>-1</v>
       </c>
@@ -3219,545 +3285,573 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="14.4">
-      <c r="A88" s="101" t="s">
-        <v>120</v>
-      </c>
-      <c r="B88" s="102"/>
-      <c r="C88" s="102"/>
-      <c r="D88" s="102"/>
-      <c r="E88" s="102"/>
-      <c r="F88" s="102"/>
-      <c r="G88" s="102"/>
-      <c r="H88" s="103"/>
-      <c r="I88" s="18">
-        <f>1.4+(-0.03*(SUM(I80:I87)))</f>
+    <row r="88" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A88" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="B88" s="82" t="s">
+        <v>81</v>
+      </c>
+      <c r="C88" s="82"/>
+      <c r="D88" s="82"/>
+      <c r="E88" s="82"/>
+      <c r="F88" s="82"/>
+      <c r="G88" s="40">
+        <v>-1</v>
+      </c>
+      <c r="H88" s="51">
+        <v>0</v>
+      </c>
+      <c r="I88" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J88" s="3">
+        <f>IF(H88&gt;3,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A89" s="125" t="s">
+        <v>119</v>
+      </c>
+      <c r="B89" s="126"/>
+      <c r="C89" s="126"/>
+      <c r="D89" s="126"/>
+      <c r="E89" s="126"/>
+      <c r="F89" s="126"/>
+      <c r="G89" s="126"/>
+      <c r="H89" s="127"/>
+      <c r="I89" s="18">
+        <f>1.4+(-0.03*(SUM(I81:I88)))</f>
         <v>1.4</v>
       </c>
     </row>
-    <row r="90" spans="1:10" ht="14.4">
-      <c r="A90" s="42" t="s">
-        <v>49</v>
-      </c>
-      <c r="B90" s="74">
-        <f>(B51*H72*I88)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:10" ht="14.4">
-      <c r="A91" s="12"/>
-      <c r="B91" s="13"/>
-    </row>
-    <row r="92" spans="1:10" ht="18">
-      <c r="A92" s="95" t="s">
+    <row r="91" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A91" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="B91" s="73">
+        <f>(B52*H73*I89)</f>
+        <v>10.079999999999998</v>
+      </c>
+    </row>
+    <row r="92" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A92" s="12"/>
+      <c r="B92" s="13"/>
+    </row>
+    <row r="93" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A93" s="119" t="s">
+        <v>107</v>
+      </c>
+      <c r="B93" s="120"/>
+      <c r="C93" s="120"/>
+      <c r="D93" s="120"/>
+      <c r="E93" s="120"/>
+      <c r="F93" s="120"/>
+      <c r="G93" s="120"/>
+      <c r="H93" s="120"/>
+      <c r="I93" s="120"/>
+    </row>
+    <row r="95" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A95" s="103" t="s">
+        <v>115</v>
+      </c>
+      <c r="B95" s="103"/>
+      <c r="C95" s="103"/>
+      <c r="D95" s="103"/>
+      <c r="E95" s="103"/>
+      <c r="F95" s="103"/>
+      <c r="G95" s="103"/>
+      <c r="H95" s="103"/>
+    </row>
+    <row r="96" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A96" s="70" t="s">
+        <v>71</v>
+      </c>
+      <c r="B96" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="C96" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="B92" s="96"/>
-      <c r="C92" s="96"/>
-      <c r="D92" s="96"/>
-      <c r="E92" s="96"/>
-      <c r="F92" s="96"/>
-      <c r="G92" s="96"/>
-      <c r="H92" s="96"/>
-      <c r="I92" s="96"/>
-    </row>
-    <row r="94" spans="1:10" ht="18">
-      <c r="A94" s="108" t="s">
-        <v>116</v>
-      </c>
-      <c r="B94" s="108"/>
-      <c r="C94" s="108"/>
-      <c r="D94" s="108"/>
-      <c r="E94" s="108"/>
-      <c r="F94" s="108"/>
-      <c r="G94" s="108"/>
-      <c r="H94" s="108"/>
-    </row>
-    <row r="95" spans="1:10" ht="14.4">
-      <c r="A95" s="70" t="s">
-        <v>72</v>
-      </c>
-      <c r="B95" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="C95" s="43" t="s">
+      <c r="D96" s="41" t="s">
         <v>109</v>
       </c>
-      <c r="D95" s="41" t="s">
+      <c r="E96" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="F96" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="G96" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="E95" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="F95" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="G95" s="41" t="s">
-        <v>111</v>
-      </c>
-      <c r="H95" s="66" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10" ht="14.4">
-      <c r="A96" s="42"/>
-      <c r="B96" s="75">
-        <f>B90</f>
-        <v>0</v>
-      </c>
-      <c r="C96" s="22">
+      <c r="H96" s="66" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A97" s="42"/>
+      <c r="B97" s="74">
+        <f>B91</f>
+        <v>10.079999999999998</v>
+      </c>
+      <c r="C97" s="22">
         <v>20</v>
       </c>
-      <c r="D96" s="21">
-        <f>B96*C96</f>
-        <v>0</v>
-      </c>
-      <c r="E96" s="21">
-        <f>D96/8</f>
-        <v>0</v>
-      </c>
-      <c r="F96" s="23">
-        <f>E96/20</f>
-        <v>0</v>
-      </c>
-      <c r="G96" s="48">
-        <v>50</v>
-      </c>
-      <c r="H96" s="24">
-        <f>G96*D96</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" ht="14.4">
-      <c r="A97" s="49">
-        <v>1</v>
-      </c>
-      <c r="B97" s="45"/>
-      <c r="C97" s="46"/>
       <c r="D97" s="21">
-        <f>D96/A97</f>
-        <v>0</v>
+        <f>B97*C97</f>
+        <v>201.59999999999997</v>
       </c>
       <c r="E97" s="21">
         <f>D97/8</f>
-        <v>0</v>
+        <v>25.199999999999996</v>
       </c>
       <c r="F97" s="23">
         <f>E97/20</f>
-        <v>0</v>
-      </c>
-      <c r="G97" s="44"/>
-      <c r="H97" s="40"/>
-    </row>
-    <row r="98" spans="1:9">
-      <c r="A98" s="3"/>
-      <c r="B98" s="3"/>
-      <c r="C98" s="3"/>
-      <c r="D98" s="3"/>
-      <c r="E98" s="3"/>
-      <c r="F98" s="14"/>
-      <c r="G98" s="3"/>
-      <c r="H98" s="3"/>
-    </row>
-    <row r="100" spans="1:9" ht="13.8" thickBot="1"/>
-    <row r="101" spans="1:9" ht="18">
-      <c r="A101" s="125" t="s">
+        <v>1.2599999999999998</v>
+      </c>
+      <c r="G97" s="48">
+        <v>50</v>
+      </c>
+      <c r="H97" s="24">
+        <f>G97*D97</f>
+        <v>10079.999999999998</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A98" s="49">
+        <v>1</v>
+      </c>
+      <c r="B98" s="45"/>
+      <c r="C98" s="46"/>
+      <c r="D98" s="21">
+        <f>D97/A98</f>
+        <v>201.59999999999997</v>
+      </c>
+      <c r="E98" s="21">
+        <f>D98/8</f>
+        <v>25.199999999999996</v>
+      </c>
+      <c r="F98" s="23">
+        <f>E98/20</f>
+        <v>1.2599999999999998</v>
+      </c>
+      <c r="G98" s="44"/>
+      <c r="H98" s="40"/>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A99" s="3"/>
+      <c r="B99" s="3"/>
+      <c r="C99" s="3"/>
+      <c r="D99" s="3"/>
+      <c r="E99" s="3"/>
+      <c r="F99" s="14"/>
+      <c r="G99" s="3"/>
+      <c r="H99" s="3"/>
+    </row>
+    <row r="101" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="102" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A102" s="94" t="s">
+        <v>47</v>
+      </c>
+      <c r="B102" s="95"/>
+      <c r="C102" s="95"/>
+      <c r="D102" s="95"/>
+      <c r="E102" s="95"/>
+      <c r="F102" s="95"/>
+      <c r="G102" s="95"/>
+      <c r="H102" s="95"/>
+      <c r="I102" s="96"/>
+    </row>
+    <row r="103" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A103" s="97" t="s">
+        <v>19</v>
+      </c>
+      <c r="B103" s="90"/>
+      <c r="C103" s="90"/>
+      <c r="D103" s="90"/>
+      <c r="E103" s="90"/>
+      <c r="F103" s="90"/>
+      <c r="G103" s="90"/>
+      <c r="H103" s="90"/>
+      <c r="I103" s="91"/>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A104" s="81" t="s">
+        <v>120</v>
+      </c>
+      <c r="B104" s="82"/>
+      <c r="C104" s="82"/>
+      <c r="D104" s="82"/>
+      <c r="E104" s="82"/>
+      <c r="F104" s="82"/>
+      <c r="G104" s="82"/>
+      <c r="H104" s="82"/>
+      <c r="I104" s="83"/>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A105" s="81" t="s">
+        <v>121</v>
+      </c>
+      <c r="B105" s="82"/>
+      <c r="C105" s="82"/>
+      <c r="D105" s="82"/>
+      <c r="E105" s="82"/>
+      <c r="F105" s="82"/>
+      <c r="G105" s="82"/>
+      <c r="H105" s="82"/>
+      <c r="I105" s="83"/>
+    </row>
+    <row r="106" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A106" s="98"/>
+      <c r="B106" s="99"/>
+      <c r="C106" s="99"/>
+      <c r="D106" s="99"/>
+      <c r="E106" s="99"/>
+      <c r="F106" s="100"/>
+      <c r="G106" s="84" t="s">
+        <v>20</v>
+      </c>
+      <c r="H106" s="85"/>
+      <c r="I106" s="19">
+        <f>SUM(J81:J86)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A107" s="98"/>
+      <c r="B107" s="99"/>
+      <c r="C107" s="99"/>
+      <c r="D107" s="99"/>
+      <c r="E107" s="99"/>
+      <c r="F107" s="100"/>
+      <c r="G107" s="84" t="s">
+        <v>21</v>
+      </c>
+      <c r="H107" s="85"/>
+      <c r="I107" s="19">
+        <f>SUM(J87:J88)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A108" s="98"/>
+      <c r="B108" s="99"/>
+      <c r="C108" s="99"/>
+      <c r="D108" s="99"/>
+      <c r="E108" s="99"/>
+      <c r="F108" s="100"/>
+      <c r="G108" s="84" t="s">
+        <v>22</v>
+      </c>
+      <c r="H108" s="85"/>
+      <c r="I108" s="19">
+        <f>I106+I107</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A109" s="92" t="s">
+        <v>90</v>
+      </c>
+      <c r="B109" s="93"/>
+      <c r="C109" s="93"/>
+      <c r="D109" s="93"/>
+      <c r="E109" s="93"/>
+      <c r="F109" s="93"/>
+      <c r="G109" s="93"/>
+      <c r="H109" s="93"/>
+      <c r="I109" s="20" t="str">
+        <f>C117</f>
+        <v>Reduzir a complexidade</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A110" s="89" t="s">
+        <v>116</v>
+      </c>
+      <c r="B110" s="90"/>
+      <c r="C110" s="90"/>
+      <c r="D110" s="90"/>
+      <c r="E110" s="90"/>
+      <c r="F110" s="90"/>
+      <c r="G110" s="90"/>
+      <c r="H110" s="90"/>
+      <c r="I110" s="91"/>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A111" s="106" t="s">
+        <v>23</v>
+      </c>
+      <c r="B111" s="79"/>
+      <c r="C111" s="79"/>
+      <c r="D111" s="79"/>
+      <c r="E111" s="79"/>
+      <c r="F111" s="79"/>
+      <c r="G111" s="79"/>
+      <c r="H111" s="79"/>
+      <c r="I111" s="80"/>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A112" s="78" t="s">
+        <v>102</v>
+      </c>
+      <c r="B112" s="79"/>
+      <c r="C112" s="79"/>
+      <c r="D112" s="79"/>
+      <c r="E112" s="79"/>
+      <c r="F112" s="79"/>
+      <c r="G112" s="79"/>
+      <c r="H112" s="79"/>
+      <c r="I112" s="80"/>
+    </row>
+    <row r="113" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="86" t="s">
+        <v>103</v>
+      </c>
+      <c r="B113" s="87"/>
+      <c r="C113" s="87"/>
+      <c r="D113" s="87"/>
+      <c r="E113" s="87"/>
+      <c r="F113" s="87"/>
+      <c r="G113" s="87"/>
+      <c r="H113" s="87"/>
+      <c r="I113" s="88"/>
+    </row>
+    <row r="115" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A115" s="103" t="s">
+        <v>89</v>
+      </c>
+      <c r="B115" s="103"/>
+      <c r="C115" s="103"/>
+      <c r="D115" s="103"/>
+      <c r="E115" s="103"/>
+      <c r="F115" s="103"/>
+      <c r="G115" s="103"/>
+      <c r="H115" s="103"/>
+    </row>
+    <row r="116" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A116" s="65" t="s">
+        <v>71</v>
+      </c>
+      <c r="B116" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="B101" s="126"/>
-      <c r="C101" s="126"/>
-      <c r="D101" s="126"/>
-      <c r="E101" s="126"/>
-      <c r="F101" s="126"/>
-      <c r="G101" s="126"/>
-      <c r="H101" s="126"/>
-      <c r="I101" s="127"/>
-    </row>
-    <row r="102" spans="1:9" ht="14.4">
-      <c r="A102" s="128" t="s">
-        <v>19</v>
-      </c>
-      <c r="B102" s="82"/>
-      <c r="C102" s="82"/>
-      <c r="D102" s="82"/>
-      <c r="E102" s="82"/>
-      <c r="F102" s="82"/>
-      <c r="G102" s="82"/>
-      <c r="H102" s="82"/>
-      <c r="I102" s="122"/>
-    </row>
-    <row r="103" spans="1:9">
-      <c r="A103" s="114" t="s">
-        <v>121</v>
-      </c>
-      <c r="B103" s="85"/>
-      <c r="C103" s="85"/>
-      <c r="D103" s="85"/>
-      <c r="E103" s="85"/>
-      <c r="F103" s="85"/>
-      <c r="G103" s="85"/>
-      <c r="H103" s="85"/>
-      <c r="I103" s="115"/>
-    </row>
-    <row r="104" spans="1:9">
-      <c r="A104" s="114" t="s">
-        <v>122</v>
-      </c>
-      <c r="B104" s="85"/>
-      <c r="C104" s="85"/>
-      <c r="D104" s="85"/>
-      <c r="E104" s="85"/>
-      <c r="F104" s="85"/>
-      <c r="G104" s="85"/>
-      <c r="H104" s="85"/>
-      <c r="I104" s="115"/>
-    </row>
-    <row r="105" spans="1:9" ht="14.4">
-      <c r="A105" s="129"/>
-      <c r="B105" s="130"/>
-      <c r="C105" s="130"/>
-      <c r="D105" s="130"/>
-      <c r="E105" s="130"/>
-      <c r="F105" s="131"/>
-      <c r="G105" s="116" t="s">
-        <v>20</v>
-      </c>
-      <c r="H105" s="117"/>
-      <c r="I105" s="19">
-        <f>SUM(J80:J85)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" ht="14.4">
-      <c r="A106" s="129"/>
-      <c r="B106" s="130"/>
-      <c r="C106" s="130"/>
-      <c r="D106" s="130"/>
-      <c r="E106" s="130"/>
-      <c r="F106" s="131"/>
-      <c r="G106" s="116" t="s">
-        <v>21</v>
-      </c>
-      <c r="H106" s="117"/>
-      <c r="I106" s="19">
-        <f>SUM(J86:J87)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9" ht="14.4">
-      <c r="A107" s="129"/>
-      <c r="B107" s="130"/>
-      <c r="C107" s="130"/>
-      <c r="D107" s="130"/>
-      <c r="E107" s="130"/>
-      <c r="F107" s="131"/>
-      <c r="G107" s="116" t="s">
-        <v>22</v>
-      </c>
-      <c r="H107" s="117"/>
-      <c r="I107" s="19">
-        <f>I105+I106</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9" ht="14.4">
-      <c r="A108" s="123" t="s">
-        <v>91</v>
-      </c>
-      <c r="B108" s="124"/>
-      <c r="C108" s="124"/>
-      <c r="D108" s="124"/>
-      <c r="E108" s="124"/>
-      <c r="F108" s="124"/>
-      <c r="G108" s="124"/>
-      <c r="H108" s="124"/>
-      <c r="I108" s="20" t="str">
-        <f>C116</f>
+      <c r="C116" s="43" t="s">
+        <v>111</v>
+      </c>
+      <c r="D116" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="E116" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="F116" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="G116" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="H116" s="66" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="42"/>
+      <c r="B117" s="74">
+        <f>B91</f>
+        <v>10.079999999999998</v>
+      </c>
+      <c r="C117" s="22" t="str">
+        <f>IF(I108&lt;=2,20,IF(I108&lt;5,28,"Reduzir a complexidade"))</f>
         <v>Reduzir a complexidade</v>
       </c>
-    </row>
-    <row r="109" spans="1:9" ht="14.4">
-      <c r="A109" s="121" t="s">
-        <v>117</v>
-      </c>
-      <c r="B109" s="82"/>
-      <c r="C109" s="82"/>
-      <c r="D109" s="82"/>
-      <c r="E109" s="82"/>
-      <c r="F109" s="82"/>
-      <c r="G109" s="82"/>
-      <c r="H109" s="82"/>
-      <c r="I109" s="122"/>
-    </row>
-    <row r="110" spans="1:9">
-      <c r="A110" s="111" t="s">
-        <v>23</v>
-      </c>
-      <c r="B110" s="83"/>
-      <c r="C110" s="83"/>
-      <c r="D110" s="83"/>
-      <c r="E110" s="83"/>
-      <c r="F110" s="83"/>
-      <c r="G110" s="83"/>
-      <c r="H110" s="83"/>
-      <c r="I110" s="112"/>
-    </row>
-    <row r="111" spans="1:9">
-      <c r="A111" s="113" t="s">
-        <v>103</v>
-      </c>
-      <c r="B111" s="83"/>
-      <c r="C111" s="83"/>
-      <c r="D111" s="83"/>
-      <c r="E111" s="83"/>
-      <c r="F111" s="83"/>
-      <c r="G111" s="83"/>
-      <c r="H111" s="83"/>
-      <c r="I111" s="112"/>
-    </row>
-    <row r="112" spans="1:9" ht="13.8" thickBot="1">
-      <c r="A112" s="118" t="s">
-        <v>104</v>
-      </c>
-      <c r="B112" s="119"/>
-      <c r="C112" s="119"/>
-      <c r="D112" s="119"/>
-      <c r="E112" s="119"/>
-      <c r="F112" s="119"/>
-      <c r="G112" s="119"/>
-      <c r="H112" s="119"/>
-      <c r="I112" s="120"/>
-    </row>
-    <row r="114" spans="1:8" ht="18">
-      <c r="A114" s="108" t="s">
-        <v>90</v>
-      </c>
-      <c r="B114" s="108"/>
-      <c r="C114" s="108"/>
-      <c r="D114" s="108"/>
-      <c r="E114" s="108"/>
-      <c r="F114" s="108"/>
-      <c r="G114" s="108"/>
-      <c r="H114" s="108"/>
-    </row>
-    <row r="115" spans="1:8" ht="14.4">
-      <c r="A115" s="65" t="s">
-        <v>72</v>
-      </c>
-      <c r="B115" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="C115" s="43" t="s">
-        <v>112</v>
-      </c>
-      <c r="D115" s="41" t="s">
-        <v>110</v>
-      </c>
-      <c r="E115" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="F115" s="41" t="s">
+      <c r="D117" s="22" t="str">
+        <f>IF(I108&lt;=2,20*B117,IF(I108&lt;5,28*B117,"-"))</f>
+        <v>-</v>
+      </c>
+      <c r="E117" s="22" t="str">
+        <f>IF(I108&lt;=2,20*B117/8,IF(I108&lt;5,28*B117/8,"-"))</f>
+        <v>-</v>
+      </c>
+      <c r="F117" s="25" t="str">
+        <f>IF(I108&lt;=2,20*B117/20/8,IF(I108&lt;5,28*B117/20/8,"-"))</f>
+        <v>-</v>
+      </c>
+      <c r="G117" s="27">
+        <f>G97</f>
+        <v>50</v>
+      </c>
+      <c r="H117" s="26" t="str">
+        <f>IF(I108&lt;=2,20*B117*G117,IF(I108&lt;5,28*B117*G117,"-"))</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A118" s="68">
+        <f>A98</f>
+        <v>1</v>
+      </c>
+      <c r="B118" s="45"/>
+      <c r="C118" s="46"/>
+      <c r="D118" s="22" t="str">
+        <f>IF(I108&lt;=2,20*B117/A118,IF(I108&lt;5,28*B117/A118,"-"))</f>
+        <v>-</v>
+      </c>
+      <c r="E118" s="22" t="str">
+        <f>IF(I108&lt;=2,20*B117/A118/8,IF(I108&lt;5,28*B117/A118/8,"-"))</f>
+        <v>-</v>
+      </c>
+      <c r="F118" s="25" t="str">
+        <f>IF(I108&lt;=2,20*B117/A118/20/8,IF(I108&lt;5,28*B117/A118/20/8,"-"))</f>
+        <v>-</v>
+      </c>
+      <c r="G118" s="44"/>
+      <c r="H118" s="40"/>
+    </row>
+    <row r="122" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="47"/>
+      <c r="B123" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G115" s="41" t="s">
-        <v>111</v>
-      </c>
-      <c r="H115" s="66" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8" ht="15" thickBot="1">
-      <c r="A116" s="42"/>
-      <c r="B116" s="75">
-        <f>B90</f>
-        <v>0</v>
-      </c>
-      <c r="C116" s="22" t="str">
-        <f>IF(I107&lt;=2,20,IF(I107&lt;5,28,"Reduzir a complexidade"))</f>
-        <v>Reduzir a complexidade</v>
-      </c>
-      <c r="D116" s="22" t="str">
-        <f>IF(I107&lt;=2,20*B116,IF(I107&lt;5,28*B116,"-"))</f>
-        <v>-</v>
-      </c>
-      <c r="E116" s="22" t="str">
-        <f>IF(I107&lt;=2,20*B116/8,IF(I107&lt;5,28*B116/8,"-"))</f>
-        <v>-</v>
-      </c>
-      <c r="F116" s="25" t="str">
-        <f>IF(I107&lt;=2,20*B116/20/8,IF(I107&lt;5,28*B116/20/8,"-"))</f>
-        <v>-</v>
-      </c>
-      <c r="G116" s="27">
-        <f>G96</f>
-        <v>50</v>
-      </c>
-      <c r="H116" s="26" t="str">
-        <f>IF(I107&lt;=2,20*B116*G116,IF(I107&lt;5,28*B116*G116,"-"))</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8" ht="15" thickBot="1">
-      <c r="A117" s="68">
-        <f>A97</f>
-        <v>1</v>
-      </c>
-      <c r="B117" s="45"/>
-      <c r="C117" s="46"/>
-      <c r="D117" s="22" t="str">
-        <f>IF(I107&lt;=2,20*B116/A117,IF(I107&lt;5,28*B116/A117,"-"))</f>
-        <v>-</v>
-      </c>
-      <c r="E117" s="22" t="str">
-        <f>IF(I107&lt;=2,20*B116/A117/8,IF(I107&lt;5,28*B116/A117/8,"-"))</f>
-        <v>-</v>
-      </c>
-      <c r="F117" s="25" t="str">
-        <f>IF(I107&lt;=2,20*B116/A117/20/8,IF(I107&lt;5,28*B116/A117/20/8,"-"))</f>
-        <v>-</v>
-      </c>
-      <c r="G117" s="44"/>
-      <c r="H117" s="40"/>
-    </row>
-    <row r="121" spans="1:8" ht="13.8" thickBot="1">
-      <c r="A121" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="122" spans="1:8" ht="13.8" thickBot="1">
-      <c r="A122" s="47"/>
-      <c r="B122" s="1" t="s">
+    </row>
+    <row r="124" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="50"/>
+      <c r="B124" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="123" spans="1:8" ht="13.8" thickBot="1">
-      <c r="A123" s="50"/>
-      <c r="B123" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="124" spans="1:8" ht="13.8" thickBot="1">
-      <c r="A124" s="17"/>
-      <c r="B124" s="54" t="s">
-        <v>60</v>
+    <row r="125" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="17"/>
+      <c r="B125" s="54" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="101">
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="A111:I111"/>
-    <mergeCell ref="A103:I103"/>
-    <mergeCell ref="A104:I104"/>
-    <mergeCell ref="G105:H105"/>
-    <mergeCell ref="G106:H106"/>
-    <mergeCell ref="A112:I112"/>
-    <mergeCell ref="G107:H107"/>
-    <mergeCell ref="A109:I109"/>
-    <mergeCell ref="A108:H108"/>
-    <mergeCell ref="A101:I101"/>
-    <mergeCell ref="A102:I102"/>
-    <mergeCell ref="A105:F105"/>
-    <mergeCell ref="A106:F106"/>
-    <mergeCell ref="B70:E70"/>
-    <mergeCell ref="H70:I70"/>
-    <mergeCell ref="B71:E71"/>
-    <mergeCell ref="A107:F107"/>
-    <mergeCell ref="B32:H32"/>
-    <mergeCell ref="B33:H33"/>
-    <mergeCell ref="B63:E63"/>
-    <mergeCell ref="H63:I63"/>
-    <mergeCell ref="H67:I67"/>
-    <mergeCell ref="A114:H114"/>
-    <mergeCell ref="A94:H94"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="A110:I110"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="H61:I61"/>
-    <mergeCell ref="B62:E62"/>
-    <mergeCell ref="H62:I62"/>
+  <mergeCells count="103">
+    <mergeCell ref="B68:E68"/>
     <mergeCell ref="B60:E60"/>
     <mergeCell ref="H60:I60"/>
+    <mergeCell ref="A58:I58"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="A93:I93"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="A30:I30"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B32:H32"/>
+    <mergeCell ref="B86:F86"/>
+    <mergeCell ref="B87:F87"/>
+    <mergeCell ref="B88:F88"/>
+    <mergeCell ref="A89:H89"/>
+    <mergeCell ref="B82:F82"/>
+    <mergeCell ref="B83:F83"/>
+    <mergeCell ref="A75:I75"/>
+    <mergeCell ref="A76:I76"/>
+    <mergeCell ref="A77:I77"/>
+    <mergeCell ref="B84:F84"/>
+    <mergeCell ref="B20:H20"/>
+    <mergeCell ref="B62:E62"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B59:E59"/>
+    <mergeCell ref="A54:I54"/>
+    <mergeCell ref="A55:I55"/>
     <mergeCell ref="A1:I1"/>
-    <mergeCell ref="H69:I69"/>
-    <mergeCell ref="B64:E64"/>
-    <mergeCell ref="H64:I64"/>
+    <mergeCell ref="H70:I70"/>
     <mergeCell ref="B65:E65"/>
     <mergeCell ref="H65:I65"/>
     <mergeCell ref="B66:E66"/>
     <mergeCell ref="H66:I66"/>
+    <mergeCell ref="B67:E67"/>
+    <mergeCell ref="H67:I67"/>
     <mergeCell ref="A16:I16"/>
     <mergeCell ref="B17:H17"/>
     <mergeCell ref="B18:H18"/>
     <mergeCell ref="B19:H19"/>
-    <mergeCell ref="B40:C40"/>
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="B44:C44"/>
     <mergeCell ref="B45:C45"/>
     <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B49:C49"/>
     <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="A55:I55"/>
-    <mergeCell ref="H58:I58"/>
     <mergeCell ref="A56:I56"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="A92:I92"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="A29:I29"/>
-    <mergeCell ref="B30:H30"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="A57:I57"/>
+    <mergeCell ref="A115:H115"/>
+    <mergeCell ref="A95:H95"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="A111:I111"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="H62:I62"/>
+    <mergeCell ref="B63:E63"/>
+    <mergeCell ref="H63:I63"/>
+    <mergeCell ref="B61:E61"/>
+    <mergeCell ref="H61:I61"/>
     <mergeCell ref="B85:F85"/>
-    <mergeCell ref="B86:F86"/>
-    <mergeCell ref="B87:F87"/>
-    <mergeCell ref="A88:H88"/>
+    <mergeCell ref="A78:I78"/>
+    <mergeCell ref="A79:I79"/>
+    <mergeCell ref="B80:F80"/>
     <mergeCell ref="B81:F81"/>
-    <mergeCell ref="B82:F82"/>
-    <mergeCell ref="A74:I74"/>
-    <mergeCell ref="A75:I75"/>
-    <mergeCell ref="A76:I76"/>
-    <mergeCell ref="B83:F83"/>
-    <mergeCell ref="B20:H20"/>
-    <mergeCell ref="B61:E61"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B58:E58"/>
-    <mergeCell ref="A53:I53"/>
-    <mergeCell ref="A54:I54"/>
-    <mergeCell ref="B84:F84"/>
-    <mergeCell ref="A77:I77"/>
-    <mergeCell ref="A78:I78"/>
-    <mergeCell ref="B79:F79"/>
-    <mergeCell ref="B80:F80"/>
-    <mergeCell ref="B36:C36"/>
     <mergeCell ref="B37:C37"/>
     <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B68:E68"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B69:E69"/>
+    <mergeCell ref="H69:I69"/>
+    <mergeCell ref="B70:E70"/>
+    <mergeCell ref="H72:I72"/>
+    <mergeCell ref="A73:G73"/>
+    <mergeCell ref="H73:I73"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="A112:I112"/>
+    <mergeCell ref="A104:I104"/>
+    <mergeCell ref="A105:I105"/>
+    <mergeCell ref="G106:H106"/>
+    <mergeCell ref="G107:H107"/>
+    <mergeCell ref="A113:I113"/>
+    <mergeCell ref="G108:H108"/>
+    <mergeCell ref="A110:I110"/>
+    <mergeCell ref="A109:H109"/>
+    <mergeCell ref="A102:I102"/>
+    <mergeCell ref="A103:I103"/>
+    <mergeCell ref="A106:F106"/>
+    <mergeCell ref="A107:F107"/>
+    <mergeCell ref="B71:E71"/>
+    <mergeCell ref="H71:I71"/>
+    <mergeCell ref="B72:E72"/>
+    <mergeCell ref="A108:F108"/>
+    <mergeCell ref="B33:H33"/>
+    <mergeCell ref="B34:H34"/>
+    <mergeCell ref="B64:E64"/>
+    <mergeCell ref="H64:I64"/>
     <mergeCell ref="H68:I68"/>
-    <mergeCell ref="B69:E69"/>
-    <mergeCell ref="H71:I71"/>
-    <mergeCell ref="A72:G72"/>
-    <mergeCell ref="H72:I72"/>
-    <mergeCell ref="B67:E67"/>
-    <mergeCell ref="B59:E59"/>
-    <mergeCell ref="H59:I59"/>
-    <mergeCell ref="A57:I57"/>
-    <mergeCell ref="B51:C51"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F49:F50">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F50:F51" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"5,10,15"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B23:B26">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B23:B27" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>$J$18:$J$21</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B36:C48">
-      <formula1>$I$31:$I$33</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B37:C49" xr:uid="{00000000-0002-0000-0000-000002000000}">
+      <formula1>$I$32:$I$34</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="G59:G71 H80:H87">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="G60:G72 H81:H88" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"0,1,2,3,4,5"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3765,7 +3859,7 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <cellWatches>
-    <cellWatch r="B36"/>
+    <cellWatch r="B37"/>
   </cellWatches>
 </worksheet>
 </file>
</xml_diff>